<commit_message>
add new exercises, definitions, update decks
- updated anki decks/wordlists for lesson 23. (3rd ed.)
- added new definitions to the dictionary.
- added the following exercises.

# Lesson 23 (3rd ed.)
- Kanji Vocabulary: 顔, 悲, and 怒
- Kanji Vocabulary: 違, 変, and 比
- Kanji Vocabulary: 情, 感, and 調
- Kanji Vocabulary: 査, 果, and 化
- Kanji Vocabulary: 横, 相, and 答
- Kanji Practice: Write the Readings
</commit_message>
<xml_diff>
--- a/resources/tools/wordlist_E-J/lessons-3rd/lesson-23.xlsx
+++ b/resources/tools/wordlist_E-J/lessons-3rd/lesson-23.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -997,6 +997,810 @@
         </is>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>face</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>顔|かお</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>emoticon</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>顔文字|かおもじ</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>complexion</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>顔色|かおいろ</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>smiling face</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>笑顔|えがお</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>washing one's face</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>洗顔|せんがん</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>sad</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>悲しい|かなしい</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>tragedy</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>悲劇|ひげき</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>miserable</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>悲惨な|ひさんな</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>to grieve</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>悲しむ|かなしむ</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>to get angry</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>怒る|おこる</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>anger; rage</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>怒り|いかり</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>human emotions</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>喜怒哀楽|きどあいらく</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>different</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>違う|ちがう</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>difference</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>違い|ちがい</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>to make a mistake</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>間違える|まちがえる</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>illegal</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>違法|いほう</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>violation</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>違反|いはん</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>strange</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>変な|へんな</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>tough; hectic</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>大変な|たいへんな</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>change</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>変化|へんか</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>eccentric person</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>変人|へんじん</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>to change (something)</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>変える|かえる</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>to compare</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>比べる|くらべる</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>comparison</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>比較|ひかく</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>proportion</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>比例|ひれい</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>contrast</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>対比|たいひ</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>figure of speech</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>比喩|ひゆ</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>expression</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>表情|ひょうじょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>to sympathize</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>同情する|どうじょうする</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>friendship</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>友情|ゆうじょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>information</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>情報|じょうほう</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>mercy</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>情け|なさけ</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>emotion</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>感情|かんじょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>to be moved</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>感動する|かんどうする</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>to feel</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>感じる|かんじる</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>gratitude</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>感謝|かんしゃ</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>impression</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>感想|かんそう</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>survey; research</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>調査|ちょうさ</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>to look into; to examine</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>調べる|しらべる</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>condition</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>調子|ちょうし</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>to emphasize</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>強調する|きょうちょうする</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>survey; research</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>調査|ちょうさ</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>inspection</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>検査|けんさ</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>screening</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>審査|しんさ</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>criminal investigation</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>捜査|そうさ</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>result</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>結果|けっか</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>fruit</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>果物|くだもの</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>fruit juice</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>果汁|かじゅう</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>effect</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>効果|こうか</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>to use up</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>使い果たす|つかいはたす</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>culture</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>文化|ぶんか</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>chemistry</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>化学|かがく</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>assimilation</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>同化|どうか</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>goblin; ghost</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>お化け|おばけ</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>makeup</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>化粧|けしょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>side</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>横|よこ</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>horizontal writing</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>横書き|よこがき</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>grand champion of sumo</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>横綱|よこづな</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>to traverse</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>横断する|おうだんする</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>partner</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>相手|あいて</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>prime minister</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>首相|しゅしょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>consultation</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>相談|そうだん</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>mutual</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>相互の|そうごの</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>to answer</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>答える|こたえる</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>answer</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>答え／答|こたえ</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>reply; answer</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>回答|かいとう</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>correct answer</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>正答|せいとう</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>